<commit_message>
Save materials and ar topics as tags
</commit_message>
<xml_diff>
--- a/spec/support/ec_grantee_report.xlsx
+++ b/spec/support/ec_grantee_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancahearn/software/headstart-tta/Head-Start-TTA/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0401D4-00D5-4840-93E7-ACDEB1CEDC1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3179395D-9D46-E449-9D6D-8906F5718D86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="11260" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EC GranteeV4" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -555,6 +555,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2378,393 +2381,436 @@
         <v>1</v>
       </c>
       <c r="X6" s="5">
-        <f>SUBTOTAL(9,X5:X5)</f>
+        <f t="shared" ref="X6:BC6" si="0">SUBTOTAL(9,X5:X5)</f>
         <v>0</v>
       </c>
       <c r="Y6" s="5">
-        <f>SUBTOTAL(9,Y5:Y5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z6" s="5">
-        <f>SUBTOTAL(9,Z5:Z5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA6" s="5">
-        <f>SUBTOTAL(9,AA5:AA5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB6" s="5">
-        <f>SUBTOTAL(9,AB5:AB5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC6" s="5">
-        <f>SUBTOTAL(9,AC5:AC5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD6" s="5">
-        <f>SUBTOTAL(9,AD5:AD5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE6" s="5">
-        <f>SUBTOTAL(9,AE5:AE5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF6" s="5">
-        <f>SUBTOTAL(9,AF5:AF5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG6" s="5">
-        <f>SUBTOTAL(9,AG5:AG5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH6" s="5">
-        <f>SUBTOTAL(9,AH5:AH5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI6" s="5">
-        <f>SUBTOTAL(9,AI5:AI5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="5">
-        <f>SUBTOTAL(9,AJ5:AJ5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK6" s="5">
-        <f>SUBTOTAL(9,AK5:AK5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AL6" s="5">
-        <f>SUBTOTAL(9,AL5:AL5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AM6" s="5">
-        <f>SUBTOTAL(9,AM5:AM5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AN6" s="5">
-        <f>SUBTOTAL(9,AN5:AN5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AO6" s="5">
-        <f>SUBTOTAL(9,AO5:AO5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AP6" s="5">
-        <f>SUBTOTAL(9,AP5:AP5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AQ6" s="5">
-        <f>SUBTOTAL(9,AQ5:AQ5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR6" s="5">
-        <f>SUBTOTAL(9,AR5:AR5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AS6" s="5">
-        <f>SUBTOTAL(9,AS5:AS5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AT6" s="5">
-        <f>SUBTOTAL(9,AT5:AT5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AU6" s="5">
-        <f>SUBTOTAL(9,AU5:AU5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AV6" s="5">
-        <f>SUBTOTAL(9,AV5:AV5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AW6" s="5">
-        <f>SUBTOTAL(9,AW5:AW5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AX6" s="5">
-        <f>SUBTOTAL(9,AX5:AX5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AY6" s="5">
-        <f>SUBTOTAL(9,AY5:AY5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AZ6" s="5">
-        <f>SUBTOTAL(9,AZ5:AZ5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="BA6" s="5">
-        <f>SUBTOTAL(9,BA5:BA5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="BB6" s="5">
-        <f>SUBTOTAL(9,BB5:BB5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="BC6" s="5">
-        <f>SUBTOTAL(9,BC5:BC5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="BD6" s="5">
-        <f>SUBTOTAL(9,BD5:BD5)</f>
+        <f t="shared" ref="BD6:CI6" si="1">SUBTOTAL(9,BD5:BD5)</f>
         <v>0</v>
       </c>
       <c r="BE6" s="5">
-        <f>SUBTOTAL(9,BE5:BE5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF6" s="5">
-        <f>SUBTOTAL(9,BF5:BF5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG6" s="5">
-        <f>SUBTOTAL(9,BG5:BG5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH6" s="5">
-        <f>SUBTOTAL(9,BH5:BH5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI6" s="5">
-        <f>SUBTOTAL(9,BI5:BI5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BJ6" s="5">
-        <f>SUBTOTAL(9,BJ5:BJ5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BK6" s="5">
-        <f>SUBTOTAL(9,BK5:BK5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BL6" s="5">
-        <f>SUBTOTAL(9,BL5:BL5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BM6" s="5">
-        <f>SUBTOTAL(9,BM5:BM5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BN6" s="5">
-        <f>SUBTOTAL(9,BN5:BN5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BO6" s="5">
-        <f>SUBTOTAL(9,BO5:BO5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BP6" s="5">
-        <f>SUBTOTAL(9,BP5:BP5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BQ6" s="5">
-        <f>SUBTOTAL(9,BQ5:BQ5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BR6" s="5">
-        <f>SUBTOTAL(9,BR5:BR5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BS6" s="5">
-        <f>SUBTOTAL(9,BS5:BS5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BT6" s="5">
-        <f>SUBTOTAL(9,BT5:BT5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BU6" s="5">
-        <f>SUBTOTAL(9,BU5:BU5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BV6" s="5">
-        <f>SUBTOTAL(9,BV5:BV5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BW6" s="5">
-        <f>SUBTOTAL(9,BW5:BW5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BX6" s="5">
-        <f>SUBTOTAL(9,BX5:BX5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BY6" s="5">
-        <f>SUBTOTAL(9,BY5:BY5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BZ6" s="5">
-        <f>SUBTOTAL(9,BZ5:BZ5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CA6" s="5">
-        <f>SUBTOTAL(9,CA5:CA5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CB6" s="5">
-        <f>SUBTOTAL(9,CB5:CB5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CC6" s="5">
-        <f>SUBTOTAL(9,CC5:CC5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CD6" s="5">
-        <f>SUBTOTAL(9,CD5:CD5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CE6" s="5">
-        <f>SUBTOTAL(9,CE5:CE5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CF6" s="5">
-        <f>SUBTOTAL(9,CF5:CF5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CG6" s="5">
-        <f>SUBTOTAL(9,CG5:CG5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CH6" s="5">
-        <f>SUBTOTAL(9,CH5:CH5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CI6" s="5">
-        <f>SUBTOTAL(9,CI5:CI5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ6" s="5">
-        <f>SUBTOTAL(9,CJ5:CJ5)</f>
+        <f t="shared" ref="CJ6:DO6" si="2">SUBTOTAL(9,CJ5:CJ5)</f>
         <v>0</v>
       </c>
       <c r="CK6" s="5">
-        <f>SUBTOTAL(9,CK5:CK5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CL6" s="5">
-        <f>SUBTOTAL(9,CL5:CL5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CM6" s="5">
-        <f>SUBTOTAL(9,CM5:CM5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CN6" s="5">
-        <f>SUBTOTAL(9,CN5:CN5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CO6" s="5">
-        <f>SUBTOTAL(9,CO5:CO5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CP6" s="5">
-        <f>SUBTOTAL(9,CP5:CP5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CQ6" s="5">
-        <f>SUBTOTAL(9,CQ5:CQ5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CR6" s="5">
-        <f>SUBTOTAL(9,CR5:CR5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CS6" s="5">
-        <f>SUBTOTAL(9,CS5:CS5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CT6" s="5">
-        <f>SUBTOTAL(9,CT5:CT5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CU6" s="5">
-        <f>SUBTOTAL(9,CU5:CU5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CV6" s="5">
-        <f>SUBTOTAL(9,CV5:CV5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CW6" s="5">
-        <f>SUBTOTAL(9,CW5:CW5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CX6" s="5">
-        <f>SUBTOTAL(9,CX5:CX5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CY6" s="5">
-        <f>SUBTOTAL(9,CY5:CY5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CZ6" s="5">
-        <f>SUBTOTAL(9,CZ5:CZ5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DA6" s="5">
-        <f>SUBTOTAL(9,DA5:DA5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DB6" s="5">
-        <f>SUBTOTAL(9,DB5:DB5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DC6" s="5">
-        <f>SUBTOTAL(9,DC5:DC5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DD6" s="5">
-        <f>SUBTOTAL(9,DD5:DD5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DE6" s="5">
-        <f>SUBTOTAL(9,DE5:DE5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DF6" s="5">
-        <f>SUBTOTAL(9,DF5:DF5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DG6" s="5">
-        <f>SUBTOTAL(9,DG5:DG5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DH6" s="5">
-        <f>SUBTOTAL(9,DH5:DH5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DI6" s="5">
-        <f>SUBTOTAL(9,DI5:DI5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DJ6" s="5">
-        <f>SUBTOTAL(9,DJ5:DJ5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A4:DJ5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="99">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="K1:K4"/>
-    <mergeCell ref="L1:L4"/>
-    <mergeCell ref="M1:M4"/>
-    <mergeCell ref="N1:N4"/>
-    <mergeCell ref="O1:O4"/>
-    <mergeCell ref="P1:P4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="R1:R4"/>
-    <mergeCell ref="S1:S4"/>
-    <mergeCell ref="T1:V3"/>
+    <mergeCell ref="DI2:DJ3"/>
+    <mergeCell ref="DI1:DJ1"/>
+    <mergeCell ref="DA2:DB3"/>
+    <mergeCell ref="DC2:DD3"/>
+    <mergeCell ref="DE2:DF3"/>
+    <mergeCell ref="DA1:DF1"/>
+    <mergeCell ref="DG2:DH3"/>
+    <mergeCell ref="DG1:DH1"/>
+    <mergeCell ref="CK1:CT1"/>
+    <mergeCell ref="CU2:CV3"/>
+    <mergeCell ref="CW2:CX3"/>
+    <mergeCell ref="CY2:CZ3"/>
+    <mergeCell ref="CU1:CZ1"/>
+    <mergeCell ref="CK2:CL3"/>
+    <mergeCell ref="CM2:CN3"/>
+    <mergeCell ref="CO2:CP3"/>
+    <mergeCell ref="CQ2:CR3"/>
+    <mergeCell ref="CS2:CT3"/>
+    <mergeCell ref="CC3:CD3"/>
+    <mergeCell ref="CE3:CF3"/>
+    <mergeCell ref="CA2:CF2"/>
+    <mergeCell ref="CG2:CH3"/>
+    <mergeCell ref="CI2:CJ3"/>
+    <mergeCell ref="BU3:BV3"/>
+    <mergeCell ref="BW3:BX3"/>
+    <mergeCell ref="BY3:BZ3"/>
+    <mergeCell ref="BQ2:BZ2"/>
+    <mergeCell ref="CA3:CB3"/>
+    <mergeCell ref="BK2:BL3"/>
+    <mergeCell ref="BM2:BN3"/>
+    <mergeCell ref="BO2:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="BG2:BH3"/>
+    <mergeCell ref="BG4"/>
+    <mergeCell ref="BH4"/>
+    <mergeCell ref="X1:BH1"/>
+    <mergeCell ref="BI2:BJ3"/>
+    <mergeCell ref="BI1:CJ1"/>
+    <mergeCell ref="AZ2:BF3"/>
+    <mergeCell ref="AZ4"/>
+    <mergeCell ref="BA4"/>
+    <mergeCell ref="BB4"/>
+    <mergeCell ref="BC4"/>
+    <mergeCell ref="BD4"/>
+    <mergeCell ref="BE4"/>
+    <mergeCell ref="BF4"/>
+    <mergeCell ref="AS2:AY3"/>
+    <mergeCell ref="AS4"/>
+    <mergeCell ref="AY4"/>
+    <mergeCell ref="AL2:AR3"/>
+    <mergeCell ref="AL4"/>
+    <mergeCell ref="AM4"/>
+    <mergeCell ref="AN4"/>
+    <mergeCell ref="AO4"/>
+    <mergeCell ref="AP4"/>
+    <mergeCell ref="AQ4"/>
+    <mergeCell ref="AR4"/>
+    <mergeCell ref="AT4"/>
+    <mergeCell ref="AU4"/>
+    <mergeCell ref="AV4"/>
+    <mergeCell ref="AW4"/>
+    <mergeCell ref="AX4"/>
     <mergeCell ref="W1:W4"/>
     <mergeCell ref="X2:AK3"/>
     <mergeCell ref="X4"/>
@@ -2781,69 +2827,26 @@
     <mergeCell ref="AI4"/>
     <mergeCell ref="AJ4"/>
     <mergeCell ref="AK4"/>
-    <mergeCell ref="AY4"/>
-    <mergeCell ref="AL2:AR3"/>
-    <mergeCell ref="AL4"/>
-    <mergeCell ref="AM4"/>
-    <mergeCell ref="AN4"/>
-    <mergeCell ref="AO4"/>
-    <mergeCell ref="AP4"/>
-    <mergeCell ref="AQ4"/>
-    <mergeCell ref="AR4"/>
-    <mergeCell ref="AT4"/>
-    <mergeCell ref="AU4"/>
-    <mergeCell ref="AV4"/>
-    <mergeCell ref="AW4"/>
-    <mergeCell ref="AX4"/>
-    <mergeCell ref="BG2:BH3"/>
-    <mergeCell ref="BG4"/>
-    <mergeCell ref="BH4"/>
-    <mergeCell ref="X1:BH1"/>
-    <mergeCell ref="BI2:BJ3"/>
-    <mergeCell ref="BI1:CJ1"/>
-    <mergeCell ref="AZ2:BF3"/>
-    <mergeCell ref="AZ4"/>
-    <mergeCell ref="BA4"/>
-    <mergeCell ref="BB4"/>
-    <mergeCell ref="BC4"/>
-    <mergeCell ref="BD4"/>
-    <mergeCell ref="BE4"/>
-    <mergeCell ref="BF4"/>
-    <mergeCell ref="AS2:AY3"/>
-    <mergeCell ref="AS4"/>
-    <mergeCell ref="BK2:BL3"/>
-    <mergeCell ref="BM2:BN3"/>
-    <mergeCell ref="BO2:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="BU3:BV3"/>
-    <mergeCell ref="BW3:BX3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="BQ2:BZ2"/>
-    <mergeCell ref="CA3:CB3"/>
-    <mergeCell ref="CC3:CD3"/>
-    <mergeCell ref="CE3:CF3"/>
-    <mergeCell ref="CA2:CF2"/>
-    <mergeCell ref="CG2:CH3"/>
-    <mergeCell ref="CI2:CJ3"/>
-    <mergeCell ref="CK1:CT1"/>
-    <mergeCell ref="CU2:CV3"/>
-    <mergeCell ref="CW2:CX3"/>
-    <mergeCell ref="CY2:CZ3"/>
-    <mergeCell ref="CU1:CZ1"/>
-    <mergeCell ref="CK2:CL3"/>
-    <mergeCell ref="CM2:CN3"/>
-    <mergeCell ref="CO2:CP3"/>
-    <mergeCell ref="CQ2:CR3"/>
-    <mergeCell ref="CS2:CT3"/>
-    <mergeCell ref="DI2:DJ3"/>
-    <mergeCell ref="DI1:DJ1"/>
-    <mergeCell ref="DA2:DB3"/>
-    <mergeCell ref="DC2:DD3"/>
-    <mergeCell ref="DE2:DF3"/>
-    <mergeCell ref="DA1:DF1"/>
-    <mergeCell ref="DG2:DH3"/>
-    <mergeCell ref="DG1:DH1"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="S1:S4"/>
+    <mergeCell ref="T1:V3"/>
+    <mergeCell ref="K1:K4"/>
+    <mergeCell ref="L1:L4"/>
+    <mergeCell ref="M1:M4"/>
+    <mergeCell ref="N1:N4"/>
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.1" footer="0.1"/>
@@ -2863,10 +2866,10 @@
   <dimension ref="A1:EB8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="DW8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="AQ5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="EA8" sqref="EA8"/>
+      <selection pane="bottomRight" activeCell="AW6" sqref="AW6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3375,7 +3378,7 @@
       <c r="W2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="Y2" s="8" t="s">
@@ -4560,6 +4563,12 @@
       <c r="W5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AW5">
+        <v>1</v>
+      </c>
       <c r="CO5" s="2">
         <v>0</v>
       </c>
@@ -4711,6 +4720,12 @@
       <c r="W7" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AT7">
+        <v>1</v>
+      </c>
+      <c r="AW7">
+        <v>1</v>
+      </c>
       <c r="DX7" s="2">
         <v>1</v>
       </c>
@@ -4890,7 +4905,7 @@
       </c>
       <c r="AT8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU8" s="5">
         <f t="shared" si="0"/>
@@ -4902,7 +4917,7 @@
       </c>
       <c r="AW8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX8" s="5">
         <f t="shared" si="0"/>
@@ -5222,47 +5237,53 @@
   </sheetData>
   <autoFilter ref="A4:EB7" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="112">
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="P1:P4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="R1:R4"/>
-    <mergeCell ref="S1:S4"/>
-    <mergeCell ref="T1:V3"/>
-    <mergeCell ref="K1:K4"/>
-    <mergeCell ref="L1:L4"/>
-    <mergeCell ref="M1:M4"/>
-    <mergeCell ref="N1:N4"/>
-    <mergeCell ref="O1:O4"/>
-    <mergeCell ref="AN4"/>
-    <mergeCell ref="AO4"/>
-    <mergeCell ref="AP4"/>
-    <mergeCell ref="AQ4"/>
-    <mergeCell ref="AR4"/>
-    <mergeCell ref="W1:W4"/>
-    <mergeCell ref="X2:AK3"/>
-    <mergeCell ref="X4"/>
-    <mergeCell ref="Y4"/>
-    <mergeCell ref="Z4"/>
-    <mergeCell ref="AA4"/>
-    <mergeCell ref="AB4"/>
-    <mergeCell ref="AC4"/>
-    <mergeCell ref="AD4"/>
-    <mergeCell ref="AE4"/>
-    <mergeCell ref="AF4"/>
-    <mergeCell ref="AG4"/>
-    <mergeCell ref="AH4"/>
-    <mergeCell ref="AI4"/>
-    <mergeCell ref="AJ4"/>
-    <mergeCell ref="AK4"/>
+    <mergeCell ref="EB2:EB4"/>
+    <mergeCell ref="DX1:EB1"/>
+    <mergeCell ref="DV2:DV4"/>
+    <mergeCell ref="DW2:DW4"/>
+    <mergeCell ref="DS1:DW1"/>
+    <mergeCell ref="DX2:DZ3"/>
+    <mergeCell ref="EA2:EA4"/>
+    <mergeCell ref="DN2:DP3"/>
+    <mergeCell ref="DQ2:DQ4"/>
+    <mergeCell ref="DR2:DR4"/>
+    <mergeCell ref="DJ1:DR1"/>
+    <mergeCell ref="DS2:DU3"/>
+    <mergeCell ref="DH2:DH4"/>
+    <mergeCell ref="DI2:DI4"/>
+    <mergeCell ref="DA1:DI1"/>
+    <mergeCell ref="DJ2:DK3"/>
+    <mergeCell ref="DL2:DM3"/>
+    <mergeCell ref="CZ2:CZ4"/>
+    <mergeCell ref="CO1:CZ1"/>
+    <mergeCell ref="DA2:DB3"/>
+    <mergeCell ref="DC2:DD3"/>
+    <mergeCell ref="DE2:DG3"/>
+    <mergeCell ref="CQ2:CR3"/>
+    <mergeCell ref="CS2:CT3"/>
+    <mergeCell ref="CU2:CV3"/>
+    <mergeCell ref="CW2:CX3"/>
+    <mergeCell ref="CY2:CY4"/>
+    <mergeCell ref="CJ2:CL3"/>
+    <mergeCell ref="CM2:CM4"/>
+    <mergeCell ref="CN2:CN4"/>
+    <mergeCell ref="BJ1:CN1"/>
+    <mergeCell ref="CO2:CP3"/>
+    <mergeCell ref="CB3:CC3"/>
+    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="CF3:CG3"/>
+    <mergeCell ref="CB2:CG2"/>
+    <mergeCell ref="CH2:CI3"/>
+    <mergeCell ref="BT3:BU3"/>
+    <mergeCell ref="BV3:BW3"/>
+    <mergeCell ref="BX3:BY3"/>
+    <mergeCell ref="BZ3:CA3"/>
+    <mergeCell ref="BR2:CA2"/>
+    <mergeCell ref="BJ2:BK3"/>
+    <mergeCell ref="BL2:BM3"/>
+    <mergeCell ref="BN2:BO3"/>
+    <mergeCell ref="BP2:BQ3"/>
+    <mergeCell ref="BR3:BS3"/>
     <mergeCell ref="BG2:BI3"/>
     <mergeCell ref="BG4"/>
     <mergeCell ref="BH4"/>
@@ -5287,53 +5308,47 @@
     <mergeCell ref="AL2:AR3"/>
     <mergeCell ref="AL4"/>
     <mergeCell ref="AM4"/>
-    <mergeCell ref="CJ2:CL3"/>
-    <mergeCell ref="CM2:CM4"/>
-    <mergeCell ref="CN2:CN4"/>
-    <mergeCell ref="BJ1:CN1"/>
-    <mergeCell ref="CO2:CP3"/>
-    <mergeCell ref="CB3:CC3"/>
-    <mergeCell ref="CD3:CE3"/>
-    <mergeCell ref="CF3:CG3"/>
-    <mergeCell ref="CB2:CG2"/>
-    <mergeCell ref="CH2:CI3"/>
-    <mergeCell ref="BT3:BU3"/>
-    <mergeCell ref="BV3:BW3"/>
-    <mergeCell ref="BX3:BY3"/>
-    <mergeCell ref="BZ3:CA3"/>
-    <mergeCell ref="BR2:CA2"/>
-    <mergeCell ref="BJ2:BK3"/>
-    <mergeCell ref="BL2:BM3"/>
-    <mergeCell ref="BN2:BO3"/>
-    <mergeCell ref="BP2:BQ3"/>
-    <mergeCell ref="BR3:BS3"/>
-    <mergeCell ref="DH2:DH4"/>
-    <mergeCell ref="DI2:DI4"/>
-    <mergeCell ref="DA1:DI1"/>
-    <mergeCell ref="DJ2:DK3"/>
-    <mergeCell ref="DL2:DM3"/>
-    <mergeCell ref="CZ2:CZ4"/>
-    <mergeCell ref="CO1:CZ1"/>
-    <mergeCell ref="DA2:DB3"/>
-    <mergeCell ref="DC2:DD3"/>
-    <mergeCell ref="DE2:DG3"/>
-    <mergeCell ref="CQ2:CR3"/>
-    <mergeCell ref="CS2:CT3"/>
-    <mergeCell ref="CU2:CV3"/>
-    <mergeCell ref="CW2:CX3"/>
-    <mergeCell ref="CY2:CY4"/>
-    <mergeCell ref="EB2:EB4"/>
-    <mergeCell ref="DX1:EB1"/>
-    <mergeCell ref="DV2:DV4"/>
-    <mergeCell ref="DW2:DW4"/>
-    <mergeCell ref="DS1:DW1"/>
-    <mergeCell ref="DX2:DZ3"/>
-    <mergeCell ref="EA2:EA4"/>
-    <mergeCell ref="DN2:DP3"/>
-    <mergeCell ref="DQ2:DQ4"/>
-    <mergeCell ref="DR2:DR4"/>
-    <mergeCell ref="DJ1:DR1"/>
-    <mergeCell ref="DS2:DU3"/>
+    <mergeCell ref="AN4"/>
+    <mergeCell ref="AO4"/>
+    <mergeCell ref="AP4"/>
+    <mergeCell ref="AQ4"/>
+    <mergeCell ref="AR4"/>
+    <mergeCell ref="W1:W4"/>
+    <mergeCell ref="X2:AK3"/>
+    <mergeCell ref="X4"/>
+    <mergeCell ref="Y4"/>
+    <mergeCell ref="Z4"/>
+    <mergeCell ref="AA4"/>
+    <mergeCell ref="AB4"/>
+    <mergeCell ref="AC4"/>
+    <mergeCell ref="AD4"/>
+    <mergeCell ref="AE4"/>
+    <mergeCell ref="AF4"/>
+    <mergeCell ref="AG4"/>
+    <mergeCell ref="AH4"/>
+    <mergeCell ref="AI4"/>
+    <mergeCell ref="AJ4"/>
+    <mergeCell ref="AK4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="S1:S4"/>
+    <mergeCell ref="T1:V3"/>
+    <mergeCell ref="K1:K4"/>
+    <mergeCell ref="L1:L4"/>
+    <mergeCell ref="M1:M4"/>
+    <mergeCell ref="N1:N4"/>
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.1" footer="0.1"/>

</xml_diff>